<commit_message>
Rerun analyses for misinfotext
</commit_message>
<xml_diff>
--- a/data/MisInfoText/Analysis_output/MisInfoText_POS_frequency.xlsx
+++ b/data/MisInfoText/Analysis_output/MisInfoText_POS_frequency.xlsx
@@ -7,27 +7,25 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="2007" sheetId="1" r:id="rId1"/>
-    <sheet name="2008" sheetId="2" r:id="rId2"/>
-    <sheet name="2009" sheetId="3" r:id="rId3"/>
-    <sheet name="2010" sheetId="4" r:id="rId4"/>
-    <sheet name="2011" sheetId="5" r:id="rId5"/>
-    <sheet name="2012" sheetId="6" r:id="rId6"/>
-    <sheet name="2013" sheetId="7" r:id="rId7"/>
-    <sheet name="2014" sheetId="8" r:id="rId8"/>
-    <sheet name="2015" sheetId="9" r:id="rId9"/>
-    <sheet name="2016" sheetId="10" r:id="rId10"/>
-    <sheet name="2017" sheetId="11" r:id="rId11"/>
-    <sheet name="2018" sheetId="12" r:id="rId12"/>
-    <sheet name="counts" sheetId="13" r:id="rId13"/>
-    <sheet name="proportions" sheetId="14" r:id="rId14"/>
+    <sheet name="2009" sheetId="1" r:id="rId1"/>
+    <sheet name="2010" sheetId="2" r:id="rId2"/>
+    <sheet name="2011" sheetId="3" r:id="rId3"/>
+    <sheet name="2012" sheetId="4" r:id="rId4"/>
+    <sheet name="2013" sheetId="5" r:id="rId5"/>
+    <sheet name="2014" sheetId="6" r:id="rId6"/>
+    <sheet name="2015" sheetId="7" r:id="rId7"/>
+    <sheet name="2016" sheetId="8" r:id="rId8"/>
+    <sheet name="2017" sheetId="9" r:id="rId9"/>
+    <sheet name="2018" sheetId="10" r:id="rId10"/>
+    <sheet name="counts" sheetId="11" r:id="rId11"/>
+    <sheet name="proportions" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="22">
   <si>
     <t>count</t>
   </si>
@@ -44,16 +42,16 @@
     <t>PUNCT</t>
   </si>
   <si>
-    <t>DET</t>
+    <t>VERB</t>
   </si>
   <si>
     <t>ADP</t>
   </si>
   <si>
-    <t>PROPN</t>
+    <t>DET</t>
   </si>
   <si>
-    <t>VERB</t>
+    <t>PROPN</t>
   </si>
   <si>
     <t>ADJ</t>
@@ -65,28 +63,28 @@
     <t>AUX</t>
   </si>
   <si>
-    <t>CCONJ</t>
+    <t>ADV</t>
   </si>
   <si>
     <t>PART</t>
   </si>
   <si>
+    <t>CCONJ</t>
+  </si>
+  <si>
     <t>SCONJ</t>
+  </si>
+  <si>
+    <t>NUM</t>
   </si>
   <si>
     <t>SPACE</t>
   </si>
   <si>
-    <t>ADV</t>
-  </si>
-  <si>
-    <t>NUM</t>
+    <t>X</t>
   </si>
   <si>
     <t>SYM</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
   <si>
     <t>INTJ</t>
@@ -450,7 +448,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -472,10 +470,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>26</v>
+        <v>2475</v>
       </c>
       <c r="C2">
-        <v>0.1756756756756757</v>
+        <v>0.1868065514378444</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -483,10 +481,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>19</v>
+        <v>1620</v>
       </c>
       <c r="C3">
-        <v>0.1283783783783784</v>
+        <v>0.1222733791229527</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -494,10 +492,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>16</v>
+        <v>1425</v>
       </c>
       <c r="C4">
-        <v>0.1081081081081081</v>
+        <v>0.1075552871914861</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -505,10 +503,10 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>1267</v>
       </c>
       <c r="C5">
-        <v>0.1013513513513514</v>
+        <v>0.09562985885727225</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -516,10 +514,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>15</v>
+        <v>1097</v>
       </c>
       <c r="C6">
-        <v>0.1013513513513514</v>
+        <v>0.08279870178881425</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -527,10 +525,10 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>14</v>
+        <v>1005</v>
       </c>
       <c r="C7">
-        <v>0.0945945945945946</v>
+        <v>0.07585478149294286</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -538,10 +536,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>14</v>
+        <v>942</v>
       </c>
       <c r="C8">
-        <v>0.0945945945945946</v>
+        <v>0.07109970563816137</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -549,10 +547,10 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>738</v>
       </c>
       <c r="C9">
-        <v>0.05405405405405406</v>
+        <v>0.05570231715601177</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -560,10 +558,10 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>688</v>
       </c>
       <c r="C10">
-        <v>0.0472972972972973</v>
+        <v>0.05192844742999472</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -571,10 +569,10 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>472</v>
       </c>
       <c r="C11">
-        <v>0.02702702702702703</v>
+        <v>0.03562533021360103</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -582,10 +580,10 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>394</v>
       </c>
       <c r="C12">
-        <v>0.02702702702702703</v>
+        <v>0.02973809344101442</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -593,10 +591,10 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>321</v>
       </c>
       <c r="C13">
-        <v>0.02027027027027027</v>
+        <v>0.02422824364102951</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -604,10 +602,10 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>299</v>
       </c>
       <c r="C14">
-        <v>0.01351351351351351</v>
+        <v>0.02256774096158201</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -615,10 +613,54 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>219</v>
       </c>
       <c r="C15">
-        <v>0.006756756756756757</v>
+        <v>0.01652954939995471</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>188</v>
+      </c>
+      <c r="C16">
+        <v>0.01418975016982414</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>57</v>
+      </c>
+      <c r="C17">
+        <v>0.004302211487659446</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>30</v>
+      </c>
+      <c r="C18">
+        <v>0.002264321835610235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>0.0009057287342440939</v>
       </c>
     </row>
   </sheetData>
@@ -650,87 +692,87 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>6872</v>
+        <v>8486</v>
       </c>
       <c r="C2">
-        <v>0.1768809039664359</v>
+        <v>0.1712440722429624</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>4402</v>
+        <v>5531</v>
       </c>
       <c r="C3">
-        <v>0.1133046768422949</v>
+        <v>0.111613358894158</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>4365</v>
+        <v>5482</v>
       </c>
       <c r="C4">
-        <v>0.1123523204035932</v>
+        <v>0.1106245585712844</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>3922</v>
+        <v>5267</v>
       </c>
       <c r="C5">
-        <v>0.1009497825023809</v>
+        <v>0.1062859449096963</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>3555</v>
+        <v>5151</v>
       </c>
       <c r="C6">
-        <v>0.09150343620498828</v>
+        <v>0.1039451114922813</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>3105</v>
+        <v>3938</v>
       </c>
       <c r="C7">
-        <v>0.07992072276131888</v>
+        <v>0.07946725860155383</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>2550</v>
+        <v>3288</v>
       </c>
       <c r="C8">
-        <v>0.06563537618079329</v>
+        <v>0.06635051962465947</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>2534</v>
+        <v>2991</v>
       </c>
       <c r="C9">
-        <v>0.06522354636946281</v>
+        <v>0.06035717889214005</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -738,109 +780,109 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>1907</v>
+        <v>2523</v>
       </c>
       <c r="C10">
-        <v>0.04908496563795012</v>
+        <v>0.05091312682877611</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>1387</v>
+        <v>1881</v>
       </c>
       <c r="C11">
-        <v>0.03570049676970992</v>
+        <v>0.03795782463928968</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12">
-        <v>1079</v>
+        <v>1296</v>
       </c>
       <c r="C12">
-        <v>0.02777277290159842</v>
+        <v>0.02615275956008475</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>1019</v>
+        <v>1268</v>
       </c>
       <c r="C13">
-        <v>0.02622841110910916</v>
+        <v>0.025587730804157</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>810</v>
+        <v>968</v>
       </c>
       <c r="C14">
-        <v>0.02084888419860493</v>
+        <v>0.0195338512763596</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>722</v>
+        <v>844</v>
       </c>
       <c r="C15">
-        <v>0.01858382023628736</v>
+        <v>0.01703158107153668</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>421</v>
+        <v>480</v>
       </c>
       <c r="C16">
-        <v>0.01083627191063293</v>
+        <v>0.009686207244475834</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17">
-        <v>129</v>
+        <v>88</v>
       </c>
       <c r="C17">
-        <v>0.003320377853851896</v>
+        <v>0.001775804661487236</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B18">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C18">
-        <v>0.001132531981158786</v>
+        <v>0.0009282615275956009</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19">
-        <v>0.0007207021698283184</v>
+        <v>0.0005448491575017657</v>
       </c>
     </row>
   </sheetData>
@@ -850,451 +892,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>14282</v>
-      </c>
-      <c r="C2">
-        <v>0.1734283736688079</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>9359</v>
-      </c>
-      <c r="C3">
-        <v>0.113647678838144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>8727</v>
-      </c>
-      <c r="C4">
-        <v>0.1059732122257167</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>8609</v>
-      </c>
-      <c r="C5">
-        <v>0.1045403213075737</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>8057</v>
-      </c>
-      <c r="C6">
-        <v>0.0978373061650739</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>6721</v>
-      </c>
-      <c r="C7">
-        <v>0.08161406661728456</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>5451</v>
-      </c>
-      <c r="C8">
-        <v>0.0661922745321854</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>4819</v>
-      </c>
-      <c r="C9">
-        <v>0.05851780791975811</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>4348</v>
-      </c>
-      <c r="C10">
-        <v>0.05279838739055992</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11">
-        <v>2919</v>
-      </c>
-      <c r="C11">
-        <v>0.03544583550897985</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>2271</v>
-      </c>
-      <c r="C12">
-        <v>0.02757707860256706</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>2246</v>
-      </c>
-      <c r="C13">
-        <v>0.02727350001821471</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>1658</v>
-      </c>
-      <c r="C14">
-        <v>0.02013333171424755</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15">
-        <v>1608</v>
-      </c>
-      <c r="C15">
-        <v>0.01952617454554286</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>908</v>
-      </c>
-      <c r="C16">
-        <v>0.01102597418367719</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17">
-        <v>258</v>
-      </c>
-      <c r="C17">
-        <v>0.003132930990516205</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18">
-        <v>59</v>
-      </c>
-      <c r="C18">
-        <v>0.0007164454590715353</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19">
-        <v>51</v>
-      </c>
-      <c r="C19">
-        <v>0.0006193003120787847</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>8486</v>
-      </c>
-      <c r="C2">
-        <v>0.1712440722429624</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>5531</v>
-      </c>
-      <c r="C3">
-        <v>0.111613358894158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>5482</v>
-      </c>
-      <c r="C4">
-        <v>0.1106245585712844</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>5267</v>
-      </c>
-      <c r="C5">
-        <v>0.1062859449096963</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>5151</v>
-      </c>
-      <c r="C6">
-        <v>0.1039451114922813</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>3938</v>
-      </c>
-      <c r="C7">
-        <v>0.07946725860155383</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>3288</v>
-      </c>
-      <c r="C8">
-        <v>0.06635051962465947</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>2991</v>
-      </c>
-      <c r="C9">
-        <v>0.06035717889214005</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>2523</v>
-      </c>
-      <c r="C10">
-        <v>0.05091312682877611</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11">
-        <v>1881</v>
-      </c>
-      <c r="C11">
-        <v>0.03795782463928968</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>1296</v>
-      </c>
-      <c r="C12">
-        <v>0.02615275956008475</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>1268</v>
-      </c>
-      <c r="C13">
-        <v>0.025587730804157</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>968</v>
-      </c>
-      <c r="C14">
-        <v>0.0195338512763596</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15">
-        <v>844</v>
-      </c>
-      <c r="C15">
-        <v>0.01703158107153668</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>480</v>
-      </c>
-      <c r="C16">
-        <v>0.009686207244475834</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17">
-        <v>88</v>
-      </c>
-      <c r="C17">
-        <v>0.001775804661487236</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18">
-        <v>46</v>
-      </c>
-      <c r="C18">
-        <v>0.0009282615275956009</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19">
-        <v>27</v>
-      </c>
-      <c r="C19">
-        <v>0.0005448491575017657</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1361,697 +959,591 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="1">
-        <v>2007</v>
+        <v>2009</v>
       </c>
       <c r="B2">
-        <v>26</v>
+        <v>2475</v>
       </c>
       <c r="C2">
-        <v>19</v>
+        <v>1620</v>
       </c>
       <c r="D2">
-        <v>16</v>
+        <v>1425</v>
       </c>
       <c r="E2">
-        <v>15</v>
+        <v>1267</v>
       </c>
       <c r="F2">
-        <v>15</v>
+        <v>1097</v>
       </c>
       <c r="G2">
-        <v>14</v>
+        <v>1005</v>
       </c>
       <c r="H2">
-        <v>14</v>
+        <v>942</v>
       </c>
       <c r="I2">
-        <v>8</v>
+        <v>738</v>
       </c>
       <c r="J2">
-        <v>7</v>
+        <v>688</v>
       </c>
       <c r="K2">
-        <v>4</v>
+        <v>472</v>
       </c>
       <c r="L2">
-        <v>4</v>
+        <v>394</v>
       </c>
       <c r="M2">
-        <v>3</v>
+        <v>321</v>
       </c>
       <c r="N2">
-        <v>2</v>
+        <v>299</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>219</v>
+      </c>
+      <c r="P2">
+        <v>188</v>
+      </c>
+      <c r="Q2">
+        <v>57</v>
+      </c>
+      <c r="R2">
+        <v>30</v>
+      </c>
+      <c r="S2">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="1">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="B3">
-        <v>827</v>
+        <v>2191</v>
       </c>
       <c r="C3">
-        <v>726</v>
+        <v>1279</v>
       </c>
       <c r="D3">
-        <v>388</v>
+        <v>1280</v>
       </c>
       <c r="E3">
-        <v>503</v>
+        <v>1156</v>
       </c>
       <c r="F3">
-        <v>832</v>
+        <v>957</v>
       </c>
       <c r="G3">
-        <v>513</v>
+        <v>1192</v>
       </c>
       <c r="H3">
-        <v>309</v>
+        <v>805</v>
       </c>
       <c r="I3">
-        <v>323</v>
+        <v>666</v>
       </c>
       <c r="J3">
+        <v>636</v>
+      </c>
+      <c r="K3">
+        <v>410</v>
+      </c>
+      <c r="L3">
+        <v>356</v>
+      </c>
+      <c r="M3">
+        <v>308</v>
+      </c>
+      <c r="N3">
+        <v>234</v>
+      </c>
+      <c r="O3">
         <v>245</v>
       </c>
-      <c r="K3">
-        <v>149</v>
-      </c>
-      <c r="L3">
-        <v>176</v>
-      </c>
-      <c r="M3">
-        <v>74</v>
-      </c>
-      <c r="N3">
-        <v>117</v>
-      </c>
-      <c r="O3">
-        <v>167</v>
-      </c>
       <c r="P3">
-        <v>141</v>
+        <v>96</v>
       </c>
       <c r="Q3">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="R3">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="S3">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="1">
-        <v>2009</v>
+        <v>2011</v>
       </c>
       <c r="B4">
-        <v>2475</v>
+        <v>4981</v>
       </c>
       <c r="C4">
-        <v>1620</v>
+        <v>2668</v>
       </c>
       <c r="D4">
-        <v>1097</v>
+        <v>2882</v>
       </c>
       <c r="E4">
-        <v>1267</v>
+        <v>2580</v>
       </c>
       <c r="F4">
-        <v>1005</v>
+        <v>2095</v>
       </c>
       <c r="G4">
-        <v>1425</v>
+        <v>2466</v>
       </c>
       <c r="H4">
-        <v>942</v>
+        <v>1709</v>
       </c>
       <c r="I4">
-        <v>738</v>
+        <v>1541</v>
       </c>
       <c r="J4">
-        <v>688</v>
+        <v>1313</v>
       </c>
       <c r="K4">
-        <v>321</v>
+        <v>819</v>
       </c>
       <c r="L4">
-        <v>394</v>
+        <v>724</v>
       </c>
       <c r="M4">
-        <v>299</v>
+        <v>715</v>
       </c>
       <c r="N4">
-        <v>188</v>
+        <v>456</v>
       </c>
       <c r="O4">
-        <v>472</v>
+        <v>413</v>
       </c>
       <c r="P4">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="Q4">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="R4">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="S4">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="1">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="B5">
-        <v>2191</v>
+        <v>3438</v>
       </c>
       <c r="C5">
-        <v>1279</v>
+        <v>2192</v>
       </c>
       <c r="D5">
+        <v>2009</v>
+      </c>
+      <c r="E5">
+        <v>1808</v>
+      </c>
+      <c r="F5">
+        <v>1419</v>
+      </c>
+      <c r="G5">
+        <v>2108</v>
+      </c>
+      <c r="H5">
+        <v>1201</v>
+      </c>
+      <c r="I5">
         <v>957</v>
       </c>
-      <c r="E5">
-        <v>1156</v>
-      </c>
-      <c r="F5">
-        <v>1192</v>
-      </c>
-      <c r="G5">
-        <v>1280</v>
-      </c>
-      <c r="H5">
-        <v>805</v>
-      </c>
-      <c r="I5">
-        <v>666</v>
-      </c>
       <c r="J5">
-        <v>636</v>
+        <v>891</v>
       </c>
       <c r="K5">
-        <v>308</v>
+        <v>533</v>
       </c>
       <c r="L5">
-        <v>356</v>
+        <v>511</v>
       </c>
       <c r="M5">
-        <v>234</v>
+        <v>481</v>
       </c>
       <c r="N5">
-        <v>96</v>
+        <v>333</v>
       </c>
       <c r="O5">
-        <v>410</v>
+        <v>457</v>
       </c>
       <c r="P5">
-        <v>245</v>
+        <v>121</v>
       </c>
       <c r="Q5">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="R5">
-        <v>4</v>
+        <v>127</v>
       </c>
       <c r="S5">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="1">
-        <v>2011</v>
+        <v>2013</v>
       </c>
       <c r="B6">
-        <v>4981</v>
+        <v>7034</v>
       </c>
       <c r="C6">
-        <v>2668</v>
+        <v>4079</v>
       </c>
       <c r="D6">
-        <v>2095</v>
+        <v>4261</v>
       </c>
       <c r="E6">
-        <v>2580</v>
+        <v>3630</v>
       </c>
       <c r="F6">
-        <v>2466</v>
+        <v>3144</v>
       </c>
       <c r="G6">
-        <v>2882</v>
+        <v>3065</v>
       </c>
       <c r="H6">
-        <v>1709</v>
+        <v>2576</v>
       </c>
       <c r="I6">
-        <v>1541</v>
+        <v>2620</v>
       </c>
       <c r="J6">
-        <v>1313</v>
+        <v>2168</v>
       </c>
       <c r="K6">
-        <v>715</v>
+        <v>1384</v>
       </c>
       <c r="L6">
-        <v>724</v>
+        <v>1226</v>
       </c>
       <c r="M6">
-        <v>456</v>
+        <v>1161</v>
       </c>
       <c r="N6">
-        <v>217</v>
+        <v>768</v>
       </c>
       <c r="O6">
-        <v>819</v>
+        <v>606</v>
       </c>
       <c r="P6">
-        <v>413</v>
+        <v>346</v>
       </c>
       <c r="Q6">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="R6">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="S6">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="1">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="B7">
-        <v>3438</v>
+        <v>2884</v>
       </c>
       <c r="C7">
-        <v>2192</v>
+        <v>2073</v>
       </c>
       <c r="D7">
-        <v>1419</v>
+        <v>1833</v>
       </c>
       <c r="E7">
-        <v>1808</v>
+        <v>1676</v>
       </c>
       <c r="F7">
-        <v>2108</v>
+        <v>1288</v>
       </c>
       <c r="G7">
-        <v>2009</v>
+        <v>2090</v>
       </c>
       <c r="H7">
-        <v>1201</v>
+        <v>930</v>
       </c>
       <c r="I7">
-        <v>957</v>
+        <v>807</v>
       </c>
       <c r="J7">
-        <v>891</v>
+        <v>763</v>
       </c>
       <c r="K7">
-        <v>481</v>
+        <v>450</v>
       </c>
       <c r="L7">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="M7">
-        <v>333</v>
+        <v>434</v>
       </c>
       <c r="N7">
-        <v>121</v>
+        <v>269</v>
       </c>
       <c r="O7">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="P7">
-        <v>457</v>
+        <v>279</v>
       </c>
       <c r="Q7">
-        <v>127</v>
+        <v>65</v>
       </c>
       <c r="R7">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="S7">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="1">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="B8">
-        <v>7034</v>
+        <v>4559</v>
       </c>
       <c r="C8">
-        <v>4079</v>
+        <v>2874</v>
       </c>
       <c r="D8">
-        <v>3144</v>
+        <v>2767</v>
       </c>
       <c r="E8">
-        <v>3630</v>
+        <v>2535</v>
       </c>
       <c r="F8">
-        <v>3065</v>
+        <v>2140</v>
       </c>
       <c r="G8">
-        <v>4261</v>
+        <v>2210</v>
       </c>
       <c r="H8">
-        <v>2576</v>
+        <v>1773</v>
       </c>
       <c r="I8">
-        <v>2620</v>
+        <v>1768</v>
       </c>
       <c r="J8">
-        <v>2168</v>
+        <v>1424</v>
       </c>
       <c r="K8">
-        <v>1161</v>
+        <v>827</v>
       </c>
       <c r="L8">
-        <v>1226</v>
+        <v>826</v>
       </c>
       <c r="M8">
-        <v>768</v>
+        <v>825</v>
       </c>
       <c r="N8">
-        <v>346</v>
+        <v>488</v>
       </c>
       <c r="O8">
-        <v>1384</v>
+        <v>377</v>
       </c>
       <c r="P8">
-        <v>606</v>
+        <v>455</v>
       </c>
       <c r="Q8">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="R8">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="S8">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="1">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="B9">
-        <v>2884</v>
+        <v>6872</v>
       </c>
       <c r="C9">
-        <v>2073</v>
+        <v>4365</v>
       </c>
       <c r="D9">
-        <v>1288</v>
+        <v>4402</v>
       </c>
       <c r="E9">
-        <v>1676</v>
+        <v>3922</v>
       </c>
       <c r="F9">
-        <v>2090</v>
+        <v>3105</v>
       </c>
       <c r="G9">
-        <v>1833</v>
+        <v>3555</v>
       </c>
       <c r="H9">
-        <v>930</v>
+        <v>2550</v>
       </c>
       <c r="I9">
-        <v>807</v>
+        <v>2534</v>
       </c>
       <c r="J9">
-        <v>763</v>
+        <v>1907</v>
       </c>
       <c r="K9">
-        <v>434</v>
+        <v>1387</v>
       </c>
       <c r="L9">
-        <v>508</v>
+        <v>1019</v>
       </c>
       <c r="M9">
-        <v>269</v>
+        <v>1079</v>
       </c>
       <c r="N9">
-        <v>279</v>
+        <v>810</v>
       </c>
       <c r="O9">
-        <v>450</v>
+        <v>722</v>
       </c>
       <c r="P9">
-        <v>534</v>
+        <v>421</v>
       </c>
       <c r="Q9">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="R9">
-        <v>65</v>
+        <v>129</v>
       </c>
       <c r="S9">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="1">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="B10">
-        <v>814</v>
+        <v>14282</v>
       </c>
       <c r="C10">
-        <v>440</v>
+        <v>8727</v>
       </c>
       <c r="D10">
-        <v>330</v>
+        <v>9359</v>
       </c>
       <c r="E10">
-        <v>412</v>
+        <v>8057</v>
       </c>
       <c r="F10">
+        <v>6721</v>
+      </c>
+      <c r="G10">
+        <v>8609</v>
+      </c>
+      <c r="H10">
+        <v>4819</v>
+      </c>
+      <c r="I10">
+        <v>5451</v>
+      </c>
+      <c r="J10">
+        <v>4348</v>
+      </c>
+      <c r="K10">
+        <v>2919</v>
+      </c>
+      <c r="L10">
+        <v>2271</v>
+      </c>
+      <c r="M10">
+        <v>2246</v>
+      </c>
+      <c r="N10">
+        <v>1658</v>
+      </c>
+      <c r="O10">
+        <v>1608</v>
+      </c>
+      <c r="P10">
+        <v>908</v>
+      </c>
+      <c r="Q10">
+        <v>59</v>
+      </c>
+      <c r="R10">
         <v>258</v>
       </c>
-      <c r="G10">
-        <v>515</v>
-      </c>
-      <c r="H10">
-        <v>328</v>
-      </c>
-      <c r="I10">
-        <v>373</v>
-      </c>
-      <c r="J10">
-        <v>292</v>
-      </c>
-      <c r="K10">
-        <v>142</v>
-      </c>
-      <c r="L10">
-        <v>144</v>
-      </c>
-      <c r="M10">
-        <v>111</v>
-      </c>
-      <c r="N10">
-        <v>18</v>
-      </c>
-      <c r="O10">
-        <v>151</v>
-      </c>
-      <c r="P10">
-        <v>48</v>
-      </c>
-      <c r="Q10">
-        <v>3</v>
-      </c>
-      <c r="R10">
-        <v>2</v>
-      </c>
       <c r="S10">
-        <v>3</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="1">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="B11">
-        <v>6872</v>
+        <v>8486</v>
       </c>
       <c r="C11">
-        <v>4365</v>
+        <v>5267</v>
       </c>
       <c r="D11">
-        <v>3105</v>
+        <v>5531</v>
       </c>
       <c r="E11">
-        <v>3922</v>
+        <v>5151</v>
       </c>
       <c r="F11">
-        <v>3555</v>
+        <v>3938</v>
       </c>
       <c r="G11">
-        <v>4402</v>
+        <v>5482</v>
       </c>
       <c r="H11">
-        <v>2550</v>
+        <v>2991</v>
       </c>
       <c r="I11">
-        <v>2534</v>
+        <v>3288</v>
       </c>
       <c r="J11">
-        <v>1907</v>
+        <v>2523</v>
       </c>
       <c r="K11">
-        <v>1079</v>
+        <v>1881</v>
       </c>
       <c r="L11">
-        <v>1019</v>
+        <v>1296</v>
       </c>
       <c r="M11">
-        <v>810</v>
+        <v>1268</v>
       </c>
       <c r="N11">
-        <v>421</v>
+        <v>968</v>
       </c>
       <c r="O11">
-        <v>1387</v>
+        <v>844</v>
       </c>
       <c r="P11">
-        <v>722</v>
+        <v>480</v>
       </c>
       <c r="Q11">
-        <v>129</v>
+        <v>27</v>
       </c>
       <c r="R11">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="S11">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19">
-      <c r="A12" s="1">
-        <v>2017</v>
-      </c>
-      <c r="B12">
-        <v>14282</v>
-      </c>
-      <c r="C12">
-        <v>8727</v>
-      </c>
-      <c r="D12">
-        <v>6721</v>
-      </c>
-      <c r="E12">
-        <v>8057</v>
-      </c>
-      <c r="F12">
-        <v>8609</v>
-      </c>
-      <c r="G12">
-        <v>9359</v>
-      </c>
-      <c r="H12">
-        <v>4819</v>
-      </c>
-      <c r="I12">
-        <v>5451</v>
-      </c>
-      <c r="J12">
-        <v>4348</v>
-      </c>
-      <c r="K12">
-        <v>2246</v>
-      </c>
-      <c r="L12">
-        <v>2271</v>
-      </c>
-      <c r="M12">
-        <v>1658</v>
-      </c>
-      <c r="N12">
-        <v>908</v>
-      </c>
-      <c r="O12">
-        <v>2919</v>
-      </c>
-      <c r="P12">
-        <v>1608</v>
-      </c>
-      <c r="Q12">
-        <v>258</v>
-      </c>
-      <c r="R12">
-        <v>59</v>
-      </c>
-      <c r="S12">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="1">
-        <v>2018</v>
-      </c>
-      <c r="B13">
-        <v>8486</v>
-      </c>
-      <c r="C13">
-        <v>5267</v>
-      </c>
-      <c r="D13">
-        <v>3938</v>
-      </c>
-      <c r="E13">
-        <v>5151</v>
-      </c>
-      <c r="F13">
-        <v>5482</v>
-      </c>
-      <c r="G13">
-        <v>5531</v>
-      </c>
-      <c r="H13">
-        <v>2991</v>
-      </c>
-      <c r="I13">
-        <v>3288</v>
-      </c>
-      <c r="J13">
-        <v>2523</v>
-      </c>
-      <c r="K13">
-        <v>1268</v>
-      </c>
-      <c r="L13">
-        <v>1296</v>
-      </c>
-      <c r="M13">
-        <v>968</v>
-      </c>
-      <c r="N13">
-        <v>480</v>
-      </c>
-      <c r="O13">
-        <v>1881</v>
-      </c>
-      <c r="P13">
-        <v>844</v>
-      </c>
-      <c r="Q13">
-        <v>88</v>
-      </c>
-      <c r="R13">
-        <v>27</v>
-      </c>
-      <c r="S13">
         <v>46</v>
       </c>
     </row>
@@ -2060,9 +1552,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2129,697 +1621,591 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="1">
-        <v>2007</v>
+        <v>2009</v>
       </c>
       <c r="B2">
-        <v>0.1756756756756757</v>
+        <v>0.1868065514378444</v>
       </c>
       <c r="C2">
-        <v>0.1283783783783784</v>
+        <v>0.1222733791229527</v>
       </c>
       <c r="D2">
-        <v>0.1081081081081081</v>
+        <v>0.1075552871914861</v>
       </c>
       <c r="E2">
-        <v>0.1013513513513514</v>
+        <v>0.09562985885727225</v>
       </c>
       <c r="F2">
-        <v>0.1013513513513514</v>
+        <v>0.08279870178881425</v>
       </c>
       <c r="G2">
-        <v>0.0945945945945946</v>
+        <v>0.07585478149294286</v>
       </c>
       <c r="H2">
-        <v>0.0945945945945946</v>
+        <v>0.07109970563816137</v>
       </c>
       <c r="I2">
-        <v>0.05405405405405406</v>
+        <v>0.05570231715601177</v>
       </c>
       <c r="J2">
-        <v>0.0472972972972973</v>
+        <v>0.05192844742999472</v>
       </c>
       <c r="K2">
-        <v>0.02702702702702703</v>
+        <v>0.03562533021360103</v>
       </c>
       <c r="L2">
-        <v>0.02702702702702703</v>
+        <v>0.02973809344101442</v>
       </c>
       <c r="M2">
-        <v>0.02027027027027027</v>
+        <v>0.02422824364102951</v>
       </c>
       <c r="N2">
-        <v>0.01351351351351351</v>
+        <v>0.02256774096158201</v>
       </c>
       <c r="O2">
-        <v>0.006756756756756757</v>
+        <v>0.01652954939995471</v>
+      </c>
+      <c r="P2">
+        <v>0.01418975016982414</v>
+      </c>
+      <c r="Q2">
+        <v>0.004302211487659446</v>
+      </c>
+      <c r="R2">
+        <v>0.002264321835610235</v>
+      </c>
+      <c r="S2">
+        <v>0.0009057287342440939</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="1">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="B3">
-        <v>0.1497374615245338</v>
+        <v>0.1846918991823316</v>
       </c>
       <c r="C3">
-        <v>0.131450298750679</v>
+        <v>0.1078142122565961</v>
       </c>
       <c r="D3">
-        <v>0.07025167481441245</v>
+        <v>0.1078985079659445</v>
       </c>
       <c r="E3">
-        <v>0.09107369183414811</v>
+        <v>0.09744584000674365</v>
       </c>
       <c r="F3">
-        <v>0.1506427666123483</v>
+        <v>0.08067099384641321</v>
       </c>
       <c r="G3">
-        <v>0.09288430200977729</v>
+        <v>0.1004804855432858</v>
       </c>
       <c r="H3">
-        <v>0.05594785442694188</v>
+        <v>0.06785804602545731</v>
       </c>
       <c r="I3">
-        <v>0.05848270867282274</v>
+        <v>0.05614094242603052</v>
       </c>
       <c r="J3">
-        <v>0.04435994930291508</v>
+        <v>0.05361207114557869</v>
       </c>
       <c r="K3">
-        <v>0.02697809161687489</v>
+        <v>0.03456124083284161</v>
       </c>
       <c r="L3">
-        <v>0.0318667390910737</v>
+        <v>0.03000927252802832</v>
       </c>
       <c r="M3">
-        <v>0.01339851529965598</v>
+        <v>0.0259630784793054</v>
       </c>
       <c r="N3">
-        <v>0.02118413905486149</v>
+        <v>0.01972519598752423</v>
       </c>
       <c r="O3">
-        <v>0.03023718993300742</v>
+        <v>0.02065244879035657</v>
       </c>
       <c r="P3">
-        <v>0.02552960347637154</v>
+        <v>0.00809238809744584</v>
       </c>
       <c r="Q3">
-        <v>0.004888647474198805</v>
+        <v>0.0003371828373935767</v>
       </c>
       <c r="R3">
-        <v>0.0007242440702516748</v>
+        <v>0.003624715501980949</v>
       </c>
       <c r="S3">
-        <v>0.0003621220351258374</v>
+        <v>0.0004214785467419708</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="1">
-        <v>2009</v>
+        <v>2011</v>
       </c>
       <c r="B4">
-        <v>0.1868065514378444</v>
+        <v>0.1939264161962235</v>
       </c>
       <c r="C4">
-        <v>0.1222733791229527</v>
+        <v>0.1038738563363831</v>
       </c>
       <c r="D4">
-        <v>0.08279870178881425</v>
+        <v>0.1122055674518201</v>
       </c>
       <c r="E4">
-        <v>0.09562985885727225</v>
+        <v>0.100447732139381</v>
       </c>
       <c r="F4">
-        <v>0.07585478149294286</v>
+        <v>0.0815651158263578</v>
       </c>
       <c r="G4">
-        <v>0.1075552871914861</v>
+        <v>0.09600934397508273</v>
       </c>
       <c r="H4">
-        <v>0.07109970563816137</v>
+        <v>0.06653688923496204</v>
       </c>
       <c r="I4">
-        <v>0.05570231715601177</v>
+        <v>0.05999610667704886</v>
       </c>
       <c r="J4">
-        <v>0.05192844742999472</v>
+        <v>0.0511193303484524</v>
       </c>
       <c r="K4">
-        <v>0.02422824364102951</v>
+        <v>0.03188631496982675</v>
       </c>
       <c r="L4">
-        <v>0.02973809344101442</v>
+        <v>0.02818765816624489</v>
       </c>
       <c r="M4">
-        <v>0.02256774096158201</v>
+        <v>0.0278372591006424</v>
       </c>
       <c r="N4">
-        <v>0.01418975016982414</v>
+        <v>0.01775355265719291</v>
       </c>
       <c r="O4">
-        <v>0.03562533021360103</v>
+        <v>0.01607942378820323</v>
       </c>
       <c r="P4">
-        <v>0.01652954939995471</v>
+        <v>0.008448510803971189</v>
       </c>
       <c r="Q4">
-        <v>0.002264321835610235</v>
+        <v>0.0008175978197391473</v>
       </c>
       <c r="R4">
-        <v>0.004302211487659446</v>
+        <v>0.002608526377262994</v>
       </c>
       <c r="S4">
-        <v>0.0009057287342440939</v>
+        <v>0.0007007981312049835</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="1">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="B5">
-        <v>0.1846918991823316</v>
+        <v>0.184580693654032</v>
       </c>
       <c r="C5">
-        <v>0.1078142122565961</v>
+        <v>0.117684956512402</v>
       </c>
       <c r="D5">
-        <v>0.08067099384641321</v>
+        <v>0.1078599806721787</v>
       </c>
       <c r="E5">
-        <v>0.09744584000674365</v>
+        <v>0.09706861376570386</v>
       </c>
       <c r="F5">
-        <v>0.1004804855432858</v>
+        <v>0.07618382905615806</v>
       </c>
       <c r="G5">
-        <v>0.1078985079659445</v>
+        <v>0.1131751315365618</v>
       </c>
       <c r="H5">
-        <v>0.06785804602545731</v>
+        <v>0.06447975947600129</v>
       </c>
       <c r="I5">
-        <v>0.05614094242603052</v>
+        <v>0.05137979168903683</v>
       </c>
       <c r="J5">
-        <v>0.05361207114557869</v>
+        <v>0.04783635777944809</v>
       </c>
       <c r="K5">
-        <v>0.0259630784793054</v>
+        <v>0.02861591323955761</v>
       </c>
       <c r="L5">
-        <v>0.03000927252802832</v>
+        <v>0.02743476860302803</v>
       </c>
       <c r="M5">
-        <v>0.01972519598752423</v>
+        <v>0.02582411682594223</v>
       </c>
       <c r="N5">
-        <v>0.00809238809744584</v>
+        <v>0.01787823472565231</v>
       </c>
       <c r="O5">
-        <v>0.03456124083284161</v>
+        <v>0.0245355954042736</v>
       </c>
       <c r="P5">
-        <v>0.02065244879035657</v>
+        <v>0.006496295500912703</v>
       </c>
       <c r="Q5">
-        <v>0.003624715501980949</v>
+        <v>0.001020079458821003</v>
       </c>
       <c r="R5">
-        <v>0.0003371828373935767</v>
+        <v>0.006818425856329862</v>
       </c>
       <c r="S5">
-        <v>0.0004214785467419708</v>
+        <v>0.001127456243960056</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="1">
-        <v>2011</v>
+        <v>2013</v>
       </c>
       <c r="B6">
-        <v>0.1939264161962235</v>
+        <v>0.1840783000104679</v>
       </c>
       <c r="C6">
-        <v>0.1038738563363831</v>
+        <v>0.1067465717575631</v>
       </c>
       <c r="D6">
-        <v>0.0815651158263578</v>
+        <v>0.1115094734638333</v>
       </c>
       <c r="E6">
-        <v>0.100447732139381</v>
+        <v>0.09499633622945672</v>
       </c>
       <c r="F6">
-        <v>0.09600934397508273</v>
+        <v>0.08227781848633937</v>
       </c>
       <c r="G6">
-        <v>0.1122055674518201</v>
+        <v>0.08021040510834293</v>
       </c>
       <c r="H6">
-        <v>0.06653688923496204</v>
+        <v>0.06741337799644091</v>
       </c>
       <c r="I6">
-        <v>0.05999610667704886</v>
+        <v>0.06856484873861614</v>
       </c>
       <c r="J6">
-        <v>0.0511193303484524</v>
+        <v>0.05673610384172511</v>
       </c>
       <c r="K6">
-        <v>0.0278372591006424</v>
+        <v>0.03621898879933005</v>
       </c>
       <c r="L6">
-        <v>0.02818765816624489</v>
+        <v>0.03208416204333717</v>
       </c>
       <c r="M6">
-        <v>0.01775355265719291</v>
+        <v>0.03038312571966921</v>
       </c>
       <c r="N6">
-        <v>0.008448510803971189</v>
+        <v>0.02009839840887679</v>
       </c>
       <c r="O6">
-        <v>0.03188631496982675</v>
+        <v>0.01585889249450434</v>
       </c>
       <c r="P6">
-        <v>0.01607942378820323</v>
+        <v>0.009054747199832514</v>
       </c>
       <c r="Q6">
-        <v>0.002608526377262994</v>
+        <v>0.0007850936878467497</v>
       </c>
       <c r="R6">
-        <v>0.0008175978197391473</v>
+        <v>0.002355281063540249</v>
       </c>
       <c r="S6">
-        <v>0.0007007981312049835</v>
+        <v>0.0006280749502773998</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="1">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="B7">
-        <v>0.184580693654032</v>
+        <v>0.1700772542312909</v>
       </c>
       <c r="C7">
-        <v>0.117684956512402</v>
+        <v>0.1222503980656956</v>
       </c>
       <c r="D7">
-        <v>0.07618382905615806</v>
+        <v>0.1080969511116353</v>
       </c>
       <c r="E7">
-        <v>0.09706861376570386</v>
+        <v>0.09883823789585422</v>
       </c>
       <c r="F7">
-        <v>0.1131751315365618</v>
+        <v>0.07595683198679011</v>
       </c>
       <c r="G7">
-        <v>0.1078599806721787</v>
+        <v>0.1232529338916082</v>
       </c>
       <c r="H7">
-        <v>0.06447975947600129</v>
+        <v>0.05484460694698354</v>
       </c>
       <c r="I7">
-        <v>0.05137979168903683</v>
+        <v>0.04759096538302766</v>
       </c>
       <c r="J7">
-        <v>0.04783635777944809</v>
+        <v>0.04499616677478328</v>
       </c>
       <c r="K7">
-        <v>0.02582411682594223</v>
+        <v>0.02653771303886301</v>
       </c>
       <c r="L7">
-        <v>0.02743476860302803</v>
+        <v>0.02995812938609424</v>
       </c>
       <c r="M7">
-        <v>0.01787823472565231</v>
+        <v>0.02559414990859232</v>
       </c>
       <c r="N7">
-        <v>0.006496295500912703</v>
+        <v>0.01586365512767588</v>
       </c>
       <c r="O7">
-        <v>0.02861591323955761</v>
+        <v>0.0314914194727841</v>
       </c>
       <c r="P7">
-        <v>0.0245355954042736</v>
+        <v>0.01645338208409506</v>
       </c>
       <c r="Q7">
-        <v>0.006818425856329862</v>
+        <v>0.003833225216724656</v>
       </c>
       <c r="R7">
-        <v>0.001020079458821003</v>
+        <v>0.003715279825440821</v>
       </c>
       <c r="S7">
-        <v>0.001127456243960056</v>
+        <v>0.0006486996520610957</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="1">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="B8">
-        <v>0.1840783000104679</v>
+        <v>0.1757381851823298</v>
       </c>
       <c r="C8">
-        <v>0.1067465717575631</v>
+        <v>0.110785598643127</v>
       </c>
       <c r="D8">
-        <v>0.08227781848633937</v>
+        <v>0.1066610130290648</v>
       </c>
       <c r="E8">
-        <v>0.09499633622945672</v>
+        <v>0.09771798627707964</v>
       </c>
       <c r="F8">
-        <v>0.08021040510834293</v>
+        <v>0.08249171228124277</v>
       </c>
       <c r="G8">
-        <v>0.1115094734638333</v>
+        <v>0.08519003931847968</v>
       </c>
       <c r="H8">
-        <v>0.06741337799644091</v>
+        <v>0.06834476910030067</v>
       </c>
       <c r="I8">
-        <v>0.06856484873861614</v>
+        <v>0.06815203145478375</v>
       </c>
       <c r="J8">
-        <v>0.05673610384172511</v>
+        <v>0.05489168144321949</v>
       </c>
       <c r="K8">
-        <v>0.03038312571966921</v>
+        <v>0.03187880656849896</v>
       </c>
       <c r="L8">
-        <v>0.03208416204333717</v>
+        <v>0.03184025903939557</v>
       </c>
       <c r="M8">
-        <v>0.02009839840887679</v>
+        <v>0.03180171151029219</v>
       </c>
       <c r="N8">
-        <v>0.009054747199832514</v>
+        <v>0.01881119420245162</v>
       </c>
       <c r="O8">
-        <v>0.03621898879933005</v>
+        <v>0.01453241847197595</v>
       </c>
       <c r="P8">
-        <v>0.01585889249450434</v>
+        <v>0.01753912574203994</v>
       </c>
       <c r="Q8">
-        <v>0.002355281063540249</v>
+        <v>0.0008094981111710739</v>
       </c>
       <c r="R8">
-        <v>0.0007850936878467497</v>
+        <v>0.002004471513375993</v>
       </c>
       <c r="S8">
-        <v>0.0006280749502773998</v>
+        <v>0.0008094981111710739</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="1">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="B9">
-        <v>0.1700772542312909</v>
+        <v>0.1768809039664359</v>
       </c>
       <c r="C9">
-        <v>0.1222503980656956</v>
+        <v>0.1123523204035932</v>
       </c>
       <c r="D9">
-        <v>0.07595683198679011</v>
+        <v>0.1133046768422949</v>
       </c>
       <c r="E9">
-        <v>0.09883823789585422</v>
+        <v>0.1009497825023809</v>
       </c>
       <c r="F9">
-        <v>0.1232529338916082</v>
+        <v>0.07992072276131888</v>
       </c>
       <c r="G9">
-        <v>0.1080969511116353</v>
+        <v>0.09150343620498828</v>
       </c>
       <c r="H9">
-        <v>0.05484460694698354</v>
+        <v>0.06563537618079329</v>
       </c>
       <c r="I9">
-        <v>0.04759096538302766</v>
+        <v>0.06522354636946281</v>
       </c>
       <c r="J9">
-        <v>0.04499616677478328</v>
+        <v>0.04908496563795012</v>
       </c>
       <c r="K9">
-        <v>0.02559414990859232</v>
+        <v>0.03570049676970992</v>
       </c>
       <c r="L9">
-        <v>0.02995812938609424</v>
+        <v>0.02622841110910916</v>
       </c>
       <c r="M9">
-        <v>0.01586365512767588</v>
+        <v>0.02777277290159842</v>
       </c>
       <c r="N9">
-        <v>0.01645338208409506</v>
+        <v>0.02084888419860493</v>
       </c>
       <c r="O9">
-        <v>0.02653771303886301</v>
+        <v>0.01858382023628736</v>
       </c>
       <c r="P9">
-        <v>0.0314914194727841</v>
+        <v>0.01083627191063293</v>
       </c>
       <c r="Q9">
-        <v>0.003715279825440821</v>
+        <v>0.001132531981158786</v>
       </c>
       <c r="R9">
-        <v>0.003833225216724656</v>
+        <v>0.003320377853851896</v>
       </c>
       <c r="S9">
-        <v>0.0006486996520610957</v>
+        <v>0.0007207021698283184</v>
       </c>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="1">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="B10">
-        <v>0.1856751824817518</v>
+        <v>0.1734283736688079</v>
       </c>
       <c r="C10">
-        <v>0.1003649635036496</v>
+        <v>0.1059732122257167</v>
       </c>
       <c r="D10">
-        <v>0.07527372262773722</v>
+        <v>0.113647678838144</v>
       </c>
       <c r="E10">
-        <v>0.09397810218978102</v>
+        <v>0.0978373061650739</v>
       </c>
       <c r="F10">
-        <v>0.05885036496350365</v>
+        <v>0.08161406661728456</v>
       </c>
       <c r="G10">
-        <v>0.1174726277372263</v>
+        <v>0.1045403213075737</v>
       </c>
       <c r="H10">
-        <v>0.07481751824817519</v>
+        <v>0.05851780791975811</v>
       </c>
       <c r="I10">
-        <v>0.08508211678832117</v>
+        <v>0.0661922745321854</v>
       </c>
       <c r="J10">
-        <v>0.0666058394160584</v>
+        <v>0.05279838739055992</v>
       </c>
       <c r="K10">
-        <v>0.03239051094890511</v>
+        <v>0.03544583550897985</v>
       </c>
       <c r="L10">
-        <v>0.03284671532846715</v>
+        <v>0.02757707860256706</v>
       </c>
       <c r="M10">
-        <v>0.02531934306569343</v>
+        <v>0.02727350001821471</v>
       </c>
       <c r="N10">
-        <v>0.004105839416058394</v>
+        <v>0.02013333171424755</v>
       </c>
       <c r="O10">
-        <v>0.03444343065693431</v>
+        <v>0.01952617454554286</v>
       </c>
       <c r="P10">
-        <v>0.01094890510948905</v>
+        <v>0.01102597418367719</v>
       </c>
       <c r="Q10">
-        <v>0.0006843065693430657</v>
+        <v>0.0007164454590715353</v>
       </c>
       <c r="R10">
-        <v>0.0004562043795620438</v>
+        <v>0.003132930990516205</v>
       </c>
       <c r="S10">
-        <v>0.0006843065693430657</v>
+        <v>0.0006193003120787847</v>
       </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="1">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="B11">
-        <v>0.1768809039664359</v>
+        <v>0.1712440722429624</v>
       </c>
       <c r="C11">
-        <v>0.1123523204035932</v>
+        <v>0.1062859449096963</v>
       </c>
       <c r="D11">
-        <v>0.07992072276131888</v>
+        <v>0.111613358894158</v>
       </c>
       <c r="E11">
-        <v>0.1009497825023809</v>
+        <v>0.1039451114922813</v>
       </c>
       <c r="F11">
-        <v>0.09150343620498828</v>
+        <v>0.07946725860155383</v>
       </c>
       <c r="G11">
-        <v>0.1133046768422949</v>
+        <v>0.1106245585712844</v>
       </c>
       <c r="H11">
-        <v>0.06563537618079329</v>
+        <v>0.06035717889214005</v>
       </c>
       <c r="I11">
-        <v>0.06522354636946281</v>
+        <v>0.06635051962465947</v>
       </c>
       <c r="J11">
-        <v>0.04908496563795012</v>
+        <v>0.05091312682877611</v>
       </c>
       <c r="K11">
-        <v>0.02777277290159842</v>
+        <v>0.03795782463928968</v>
       </c>
       <c r="L11">
-        <v>0.02622841110910916</v>
+        <v>0.02615275956008475</v>
       </c>
       <c r="M11">
-        <v>0.02084888419860493</v>
+        <v>0.025587730804157</v>
       </c>
       <c r="N11">
-        <v>0.01083627191063293</v>
+        <v>0.0195338512763596</v>
       </c>
       <c r="O11">
-        <v>0.03570049676970992</v>
+        <v>0.01703158107153668</v>
       </c>
       <c r="P11">
-        <v>0.01858382023628736</v>
+        <v>0.009686207244475834</v>
       </c>
       <c r="Q11">
-        <v>0.003320377853851896</v>
+        <v>0.0005448491575017657</v>
       </c>
       <c r="R11">
-        <v>0.001132531981158786</v>
+        <v>0.001775804661487236</v>
       </c>
       <c r="S11">
-        <v>0.0007207021698283184</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19">
-      <c r="A12" s="1">
-        <v>2017</v>
-      </c>
-      <c r="B12">
-        <v>0.1734283736688079</v>
-      </c>
-      <c r="C12">
-        <v>0.1059732122257167</v>
-      </c>
-      <c r="D12">
-        <v>0.08161406661728456</v>
-      </c>
-      <c r="E12">
-        <v>0.0978373061650739</v>
-      </c>
-      <c r="F12">
-        <v>0.1045403213075737</v>
-      </c>
-      <c r="G12">
-        <v>0.113647678838144</v>
-      </c>
-      <c r="H12">
-        <v>0.05851780791975811</v>
-      </c>
-      <c r="I12">
-        <v>0.0661922745321854</v>
-      </c>
-      <c r="J12">
-        <v>0.05279838739055992</v>
-      </c>
-      <c r="K12">
-        <v>0.02727350001821471</v>
-      </c>
-      <c r="L12">
-        <v>0.02757707860256706</v>
-      </c>
-      <c r="M12">
-        <v>0.02013333171424755</v>
-      </c>
-      <c r="N12">
-        <v>0.01102597418367719</v>
-      </c>
-      <c r="O12">
-        <v>0.03544583550897985</v>
-      </c>
-      <c r="P12">
-        <v>0.01952617454554286</v>
-      </c>
-      <c r="Q12">
-        <v>0.003132930990516205</v>
-      </c>
-      <c r="R12">
-        <v>0.0007164454590715353</v>
-      </c>
-      <c r="S12">
-        <v>0.0006193003120787847</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="1">
-        <v>2018</v>
-      </c>
-      <c r="B13">
-        <v>0.1712440722429624</v>
-      </c>
-      <c r="C13">
-        <v>0.1062859449096963</v>
-      </c>
-      <c r="D13">
-        <v>0.07946725860155383</v>
-      </c>
-      <c r="E13">
-        <v>0.1039451114922813</v>
-      </c>
-      <c r="F13">
-        <v>0.1106245585712844</v>
-      </c>
-      <c r="G13">
-        <v>0.111613358894158</v>
-      </c>
-      <c r="H13">
-        <v>0.06035717889214005</v>
-      </c>
-      <c r="I13">
-        <v>0.06635051962465947</v>
-      </c>
-      <c r="J13">
-        <v>0.05091312682877611</v>
-      </c>
-      <c r="K13">
-        <v>0.025587730804157</v>
-      </c>
-      <c r="L13">
-        <v>0.02615275956008475</v>
-      </c>
-      <c r="M13">
-        <v>0.0195338512763596</v>
-      </c>
-      <c r="N13">
-        <v>0.009686207244475834</v>
-      </c>
-      <c r="O13">
-        <v>0.03795782463928968</v>
-      </c>
-      <c r="P13">
-        <v>0.01703158107153668</v>
-      </c>
-      <c r="Q13">
-        <v>0.001775804661487236</v>
-      </c>
-      <c r="R13">
-        <v>0.0005448491575017657</v>
-      </c>
-      <c r="S13">
         <v>0.0009282615275956009</v>
       </c>
     </row>
@@ -2849,24 +2235,24 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>832</v>
+        <v>2191</v>
       </c>
       <c r="C2">
-        <v>0.1506427666123483</v>
+        <v>0.1846918991823316</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>827</v>
+        <v>1280</v>
       </c>
       <c r="C3">
-        <v>0.1497374615245338</v>
+        <v>0.1078985079659445</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2874,10 +2260,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>726</v>
+        <v>1279</v>
       </c>
       <c r="C4">
-        <v>0.131450298750679</v>
+        <v>0.1078142122565961</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2885,10 +2271,10 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>513</v>
+        <v>1192</v>
       </c>
       <c r="C5">
-        <v>0.09288430200977729</v>
+        <v>0.1004804855432858</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2896,43 +2282,43 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>503</v>
+        <v>1156</v>
       </c>
       <c r="C6">
-        <v>0.09107369183414811</v>
+        <v>0.09744584000674365</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>388</v>
+        <v>957</v>
       </c>
       <c r="C7">
-        <v>0.07025167481441245</v>
+        <v>0.08067099384641321</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>323</v>
+        <v>805</v>
       </c>
       <c r="C8">
-        <v>0.05848270867282274</v>
+        <v>0.06785804602545731</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>309</v>
+        <v>666</v>
       </c>
       <c r="C9">
-        <v>0.05594785442694188</v>
+        <v>0.05614094242603052</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2940,54 +2326,54 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>245</v>
+        <v>636</v>
       </c>
       <c r="C10">
-        <v>0.04435994930291508</v>
+        <v>0.05361207114557869</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>176</v>
+        <v>410</v>
       </c>
       <c r="C11">
-        <v>0.0318667390910737</v>
+        <v>0.03456124083284161</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B12">
-        <v>167</v>
+        <v>356</v>
       </c>
       <c r="C12">
-        <v>0.03023718993300742</v>
+        <v>0.03000927252802832</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>149</v>
+        <v>308</v>
       </c>
       <c r="C13">
-        <v>0.02697809161687489</v>
+        <v>0.0259630784793054</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
-        <v>141</v>
+        <v>245</v>
       </c>
       <c r="C14">
-        <v>0.02552960347637154</v>
+        <v>0.02065244879035657</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2995,54 +2381,54 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>117</v>
+        <v>234</v>
       </c>
       <c r="C15">
-        <v>0.02118413905486149</v>
+        <v>0.01972519598752423</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="C16">
-        <v>0.01339851529965598</v>
+        <v>0.00809238809744584</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C17">
-        <v>0.004888647474198805</v>
+        <v>0.003624715501980949</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C18">
-        <v>0.0007242440702516748</v>
+        <v>0.0004214785467419708</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C19">
-        <v>0.0003621220351258374</v>
+        <v>0.0003371828373935767</v>
       </c>
     </row>
   </sheetData>
@@ -3074,32 +2460,32 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>2475</v>
+        <v>4981</v>
       </c>
       <c r="C2">
-        <v>0.1868065514378444</v>
+        <v>0.1939264161962235</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>1620</v>
+        <v>2882</v>
       </c>
       <c r="C3">
-        <v>0.1222733791229527</v>
+        <v>0.1122055674518201</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>1425</v>
+        <v>2668</v>
       </c>
       <c r="C4">
-        <v>0.1075552871914861</v>
+        <v>0.1038738563363831</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3107,21 +2493,21 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>1267</v>
+        <v>2580</v>
       </c>
       <c r="C5">
-        <v>0.09562985885727225</v>
+        <v>0.100447732139381</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>1097</v>
+        <v>2466</v>
       </c>
       <c r="C6">
-        <v>0.08279870178881425</v>
+        <v>0.09600934397508273</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3129,10 +2515,10 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>1005</v>
+        <v>2095</v>
       </c>
       <c r="C7">
-        <v>0.07585478149294286</v>
+        <v>0.0815651158263578</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3140,10 +2526,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>942</v>
+        <v>1709</v>
       </c>
       <c r="C8">
-        <v>0.07109970563816137</v>
+        <v>0.06653688923496204</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3151,10 +2537,10 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>738</v>
+        <v>1541</v>
       </c>
       <c r="C9">
-        <v>0.05570231715601177</v>
+        <v>0.05999610667704886</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3162,21 +2548,21 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>688</v>
+        <v>1313</v>
       </c>
       <c r="C10">
-        <v>0.05192844742999472</v>
+        <v>0.0511193303484524</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>472</v>
+        <v>819</v>
       </c>
       <c r="C11">
-        <v>0.03562533021360103</v>
+        <v>0.03188631496982675</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3184,54 +2570,54 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>394</v>
+        <v>724</v>
       </c>
       <c r="C12">
-        <v>0.02973809344101442</v>
+        <v>0.02818765816624489</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>321</v>
+        <v>715</v>
       </c>
       <c r="C13">
-        <v>0.02422824364102951</v>
+        <v>0.0278372591006424</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>299</v>
+        <v>456</v>
       </c>
       <c r="C14">
-        <v>0.02256774096158201</v>
+        <v>0.01775355265719291</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>219</v>
+        <v>413</v>
       </c>
       <c r="C15">
-        <v>0.01652954939995471</v>
+        <v>0.01607942378820323</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>188</v>
+        <v>217</v>
       </c>
       <c r="C16">
-        <v>0.01418975016982414</v>
+        <v>0.008448510803971189</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -3239,10 +2625,10 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C17">
-        <v>0.004302211487659446</v>
+        <v>0.002608526377262994</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -3250,10 +2636,10 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C18">
-        <v>0.002264321835610235</v>
+        <v>0.0008175978197391473</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -3261,10 +2647,10 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C19">
-        <v>0.0009057287342440939</v>
+        <v>0.0007007981312049835</v>
       </c>
     </row>
   </sheetData>
@@ -3296,43 +2682,43 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>2191</v>
+        <v>3438</v>
       </c>
       <c r="C2">
-        <v>0.1846918991823316</v>
+        <v>0.184580693654032</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>1280</v>
+        <v>2192</v>
       </c>
       <c r="C3">
-        <v>0.1078985079659445</v>
+        <v>0.117684956512402</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>1279</v>
+        <v>2108</v>
       </c>
       <c r="C4">
-        <v>0.1078142122565961</v>
+        <v>0.1131751315365618</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>1192</v>
+        <v>2009</v>
       </c>
       <c r="C5">
-        <v>0.1004804855432858</v>
+        <v>0.1078599806721787</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3340,21 +2726,21 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>1156</v>
+        <v>1808</v>
       </c>
       <c r="C6">
-        <v>0.09744584000674365</v>
+        <v>0.09706861376570386</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>957</v>
+        <v>1419</v>
       </c>
       <c r="C7">
-        <v>0.08067099384641321</v>
+        <v>0.07618382905615806</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3362,10 +2748,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>805</v>
+        <v>1201</v>
       </c>
       <c r="C8">
-        <v>0.06785804602545731</v>
+        <v>0.06447975947600129</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3373,10 +2759,10 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>666</v>
+        <v>957</v>
       </c>
       <c r="C9">
-        <v>0.05614094242603052</v>
+        <v>0.05137979168903683</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3384,21 +2770,21 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>636</v>
+        <v>891</v>
       </c>
       <c r="C10">
-        <v>0.05361207114557869</v>
+        <v>0.04783635777944809</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>410</v>
+        <v>533</v>
       </c>
       <c r="C11">
-        <v>0.03456124083284161</v>
+        <v>0.02861591323955761</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3406,65 +2792,65 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>356</v>
+        <v>511</v>
       </c>
       <c r="C12">
-        <v>0.03000927252802832</v>
+        <v>0.02743476860302803</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>308</v>
+        <v>481</v>
       </c>
       <c r="C13">
-        <v>0.0259630784793054</v>
+        <v>0.02582411682594223</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
-        <v>245</v>
+        <v>457</v>
       </c>
       <c r="C14">
-        <v>0.02065244879035657</v>
+        <v>0.0245355954042736</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>234</v>
+        <v>333</v>
       </c>
       <c r="C15">
-        <v>0.01972519598752423</v>
+        <v>0.01787823472565231</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B16">
-        <v>96</v>
+        <v>127</v>
       </c>
       <c r="C16">
-        <v>0.00809238809744584</v>
+        <v>0.006818425856329862</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>43</v>
+        <v>121</v>
       </c>
       <c r="C17">
-        <v>0.003624715501980949</v>
+        <v>0.006496295500912703</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -3472,21 +2858,21 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C18">
-        <v>0.0004214785467419708</v>
+        <v>0.001127456243960056</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
         <v>19</v>
       </c>
-      <c r="B19">
-        <v>4</v>
-      </c>
       <c r="C19">
-        <v>0.0003371828373935767</v>
+        <v>0.001020079458821003</v>
       </c>
     </row>
   </sheetData>
@@ -3518,21 +2904,21 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>4981</v>
+        <v>7034</v>
       </c>
       <c r="C2">
-        <v>0.1939264161962235</v>
+        <v>0.1840783000104679</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>2882</v>
+        <v>4261</v>
       </c>
       <c r="C3">
-        <v>0.1122055674518201</v>
+        <v>0.1115094734638333</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3540,10 +2926,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>2668</v>
+        <v>4079</v>
       </c>
       <c r="C4">
-        <v>0.1038738563363831</v>
+        <v>0.1067465717575631</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3551,10 +2937,10 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>2580</v>
+        <v>3630</v>
       </c>
       <c r="C5">
-        <v>0.100447732139381</v>
+        <v>0.09499633622945672</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3562,43 +2948,43 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>2466</v>
+        <v>3144</v>
       </c>
       <c r="C6">
-        <v>0.09600934397508273</v>
+        <v>0.08227781848633937</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>2095</v>
+        <v>3065</v>
       </c>
       <c r="C7">
-        <v>0.0815651158263578</v>
+        <v>0.08021040510834293</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>1709</v>
+        <v>2620</v>
       </c>
       <c r="C8">
-        <v>0.06653688923496204</v>
+        <v>0.06856484873861614</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>1541</v>
+        <v>2576</v>
       </c>
       <c r="C9">
-        <v>0.05999610667704886</v>
+        <v>0.06741337799644091</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3606,21 +2992,21 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>1313</v>
+        <v>2168</v>
       </c>
       <c r="C10">
-        <v>0.0511193303484524</v>
+        <v>0.05673610384172511</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>819</v>
+        <v>1384</v>
       </c>
       <c r="C11">
-        <v>0.03188631496982675</v>
+        <v>0.03621898879933005</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3628,76 +3014,76 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>724</v>
+        <v>1226</v>
       </c>
       <c r="C12">
-        <v>0.02818765816624489</v>
+        <v>0.03208416204333717</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>715</v>
+        <v>1161</v>
       </c>
       <c r="C13">
-        <v>0.0278372591006424</v>
+        <v>0.03038312571966921</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>456</v>
+        <v>768</v>
       </c>
       <c r="C14">
-        <v>0.01775355265719291</v>
+        <v>0.02009839840887679</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>413</v>
+        <v>606</v>
       </c>
       <c r="C15">
-        <v>0.01607942378820323</v>
+        <v>0.01585889249450434</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>217</v>
+        <v>346</v>
       </c>
       <c r="C16">
-        <v>0.008448510803971189</v>
+        <v>0.009054747199832514</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="C17">
-        <v>0.002608526377262994</v>
+        <v>0.002355281063540249</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C18">
-        <v>0.0008175978197391473</v>
+        <v>0.0007850936878467497</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -3705,10 +3091,10 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C19">
-        <v>0.0007007981312049835</v>
+        <v>0.0006280749502773998</v>
       </c>
     </row>
   </sheetData>
@@ -3740,43 +3126,43 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>3438</v>
+        <v>2884</v>
       </c>
       <c r="C2">
-        <v>0.184580693654032</v>
+        <v>0.1700772542312909</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>2192</v>
+        <v>2090</v>
       </c>
       <c r="C3">
-        <v>0.117684956512402</v>
+        <v>0.1232529338916082</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>2108</v>
+        <v>2073</v>
       </c>
       <c r="C4">
-        <v>0.1131751315365618</v>
+        <v>0.1222503980656956</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>2009</v>
+        <v>1833</v>
       </c>
       <c r="C5">
-        <v>0.1078599806721787</v>
+        <v>0.1080969511116353</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3784,21 +3170,21 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>1808</v>
+        <v>1676</v>
       </c>
       <c r="C6">
-        <v>0.09706861376570386</v>
+        <v>0.09883823789585422</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>1419</v>
+        <v>1288</v>
       </c>
       <c r="C7">
-        <v>0.07618382905615806</v>
+        <v>0.07595683198679011</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3806,10 +3192,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>1201</v>
+        <v>930</v>
       </c>
       <c r="C8">
-        <v>0.06447975947600129</v>
+        <v>0.05484460694698354</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3817,10 +3203,10 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>957</v>
+        <v>807</v>
       </c>
       <c r="C9">
-        <v>0.05137979168903683</v>
+        <v>0.04759096538302766</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3828,10 +3214,10 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>891</v>
+        <v>763</v>
       </c>
       <c r="C10">
-        <v>0.04783635777944809</v>
+        <v>0.04499616677478328</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3839,10 +3225,10 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C11">
-        <v>0.02861591323955761</v>
+        <v>0.0314914194727841</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3850,10 +3236,10 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C12">
-        <v>0.02743476860302803</v>
+        <v>0.02995812938609424</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -3861,76 +3247,76 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>481</v>
+        <v>450</v>
       </c>
       <c r="C13">
-        <v>0.02582411682594223</v>
+        <v>0.02653771303886301</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>457</v>
+        <v>434</v>
       </c>
       <c r="C14">
-        <v>0.0245355954042736</v>
+        <v>0.02559414990859232</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B15">
-        <v>333</v>
+        <v>279</v>
       </c>
       <c r="C15">
-        <v>0.01787823472565231</v>
+        <v>0.01645338208409506</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>127</v>
+        <v>269</v>
       </c>
       <c r="C16">
-        <v>0.006818425856329862</v>
+        <v>0.01586365512767588</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B17">
-        <v>121</v>
+        <v>65</v>
       </c>
       <c r="C17">
-        <v>0.006496295500912703</v>
+        <v>0.003833225216724656</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="C18">
-        <v>0.001127456243960056</v>
+        <v>0.003715279825440821</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C19">
-        <v>0.001020079458821003</v>
+        <v>0.0006486996520610957</v>
       </c>
     </row>
   </sheetData>
@@ -3962,32 +3348,32 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>7034</v>
+        <v>4559</v>
       </c>
       <c r="C2">
-        <v>0.1840783000104679</v>
+        <v>0.1757381851823298</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>4261</v>
+        <v>2874</v>
       </c>
       <c r="C3">
-        <v>0.1115094734638333</v>
+        <v>0.110785598643127</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>4079</v>
+        <v>2767</v>
       </c>
       <c r="C4">
-        <v>0.1067465717575631</v>
+        <v>0.1066610130290648</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3995,21 +3381,21 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>3630</v>
+        <v>2535</v>
       </c>
       <c r="C5">
-        <v>0.09499633622945672</v>
+        <v>0.09771798627707964</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>3144</v>
+        <v>2210</v>
       </c>
       <c r="C6">
-        <v>0.08227781848633937</v>
+        <v>0.08519003931847968</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -4017,32 +3403,32 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>3065</v>
+        <v>2140</v>
       </c>
       <c r="C7">
-        <v>0.08021040510834293</v>
+        <v>0.08249171228124277</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>2620</v>
+        <v>1773</v>
       </c>
       <c r="C8">
-        <v>0.06856484873861614</v>
+        <v>0.06834476910030067</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>2576</v>
+        <v>1768</v>
       </c>
       <c r="C9">
-        <v>0.06741337799644091</v>
+        <v>0.06815203145478375</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -4050,21 +3436,21 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>2168</v>
+        <v>1424</v>
       </c>
       <c r="C10">
-        <v>0.05673610384172511</v>
+        <v>0.05489168144321949</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>1384</v>
+        <v>827</v>
       </c>
       <c r="C11">
-        <v>0.03621898879933005</v>
+        <v>0.03187880656849896</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -4072,32 +3458,32 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>1226</v>
+        <v>826</v>
       </c>
       <c r="C12">
-        <v>0.03208416204333717</v>
+        <v>0.03184025903939557</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>1161</v>
+        <v>825</v>
       </c>
       <c r="C13">
-        <v>0.03038312571966921</v>
+        <v>0.03180171151029219</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>768</v>
+        <v>488</v>
       </c>
       <c r="C14">
-        <v>0.02009839840887679</v>
+        <v>0.01881119420245162</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -4105,43 +3491,43 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>606</v>
+        <v>455</v>
       </c>
       <c r="C15">
-        <v>0.01585889249450434</v>
+        <v>0.01753912574203994</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16">
-        <v>346</v>
+        <v>377</v>
       </c>
       <c r="C16">
-        <v>0.009054747199832514</v>
+        <v>0.01453241847197595</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="C17">
-        <v>0.002355281063540249</v>
+        <v>0.002004471513375993</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C18">
-        <v>0.0007850936878467497</v>
+        <v>0.0008094981111710739</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -4149,10 +3535,10 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C19">
-        <v>0.0006280749502773998</v>
+        <v>0.0008094981111710739</v>
       </c>
     </row>
   </sheetData>
@@ -4184,21 +3570,21 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>2884</v>
+        <v>6872</v>
       </c>
       <c r="C2">
-        <v>0.1700772542312909</v>
+        <v>0.1768809039664359</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>2090</v>
+        <v>4402</v>
       </c>
       <c r="C3">
-        <v>0.1232529338916082</v>
+        <v>0.1133046768422949</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -4206,43 +3592,43 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>2073</v>
+        <v>4365</v>
       </c>
       <c r="C4">
-        <v>0.1222503980656956</v>
+        <v>0.1123523204035932</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>1833</v>
+        <v>3922</v>
       </c>
       <c r="C5">
-        <v>0.1080969511116353</v>
+        <v>0.1009497825023809</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>1676</v>
+        <v>3555</v>
       </c>
       <c r="C6">
-        <v>0.09883823789585422</v>
+        <v>0.09150343620498828</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>1288</v>
+        <v>3105</v>
       </c>
       <c r="C7">
-        <v>0.07595683198679011</v>
+        <v>0.07992072276131888</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -4250,10 +3636,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>930</v>
+        <v>2550</v>
       </c>
       <c r="C8">
-        <v>0.05484460694698354</v>
+        <v>0.06563537618079329</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -4261,10 +3647,10 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>807</v>
+        <v>2534</v>
       </c>
       <c r="C9">
-        <v>0.04759096538302766</v>
+        <v>0.06522354636946281</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -4272,76 +3658,76 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>763</v>
+        <v>1907</v>
       </c>
       <c r="C10">
-        <v>0.04499616677478328</v>
+        <v>0.04908496563795012</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>534</v>
+        <v>1387</v>
       </c>
       <c r="C11">
-        <v>0.0314914194727841</v>
+        <v>0.03570049676970992</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12">
-        <v>508</v>
+        <v>1079</v>
       </c>
       <c r="C12">
-        <v>0.02995812938609424</v>
+        <v>0.02777277290159842</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>450</v>
+        <v>1019</v>
       </c>
       <c r="C13">
-        <v>0.02653771303886301</v>
+        <v>0.02622841110910916</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>434</v>
+        <v>810</v>
       </c>
       <c r="C14">
-        <v>0.02559414990859232</v>
+        <v>0.02084888419860493</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>279</v>
+        <v>722</v>
       </c>
       <c r="C15">
-        <v>0.01645338208409506</v>
+        <v>0.01858382023628736</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>269</v>
+        <v>421</v>
       </c>
       <c r="C16">
-        <v>0.01586365512767588</v>
+        <v>0.01083627191063293</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -4349,10 +3735,10 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>65</v>
+        <v>129</v>
       </c>
       <c r="C17">
-        <v>0.003833225216724656</v>
+        <v>0.003320377853851896</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -4360,10 +3746,10 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="C18">
-        <v>0.003715279825440821</v>
+        <v>0.001132531981158786</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -4371,10 +3757,10 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C19">
-        <v>0.0006486996520610957</v>
+        <v>0.0007207021698283184</v>
       </c>
     </row>
   </sheetData>
@@ -4406,21 +3792,21 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>814</v>
+        <v>14282</v>
       </c>
       <c r="C2">
-        <v>0.1856751824817518</v>
+        <v>0.1734283736688079</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>515</v>
+        <v>9359</v>
       </c>
       <c r="C3">
-        <v>0.1174726277372263</v>
+        <v>0.113647678838144</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -4428,87 +3814,87 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>440</v>
+        <v>8727</v>
       </c>
       <c r="C4">
-        <v>0.1003649635036496</v>
+        <v>0.1059732122257167</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>412</v>
+        <v>8609</v>
       </c>
       <c r="C5">
-        <v>0.09397810218978102</v>
+        <v>0.1045403213075737</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>373</v>
+        <v>8057</v>
       </c>
       <c r="C6">
-        <v>0.08508211678832117</v>
+        <v>0.0978373061650739</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>330</v>
+        <v>6721</v>
       </c>
       <c r="C7">
-        <v>0.07527372262773722</v>
+        <v>0.08161406661728456</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>328</v>
+        <v>5451</v>
       </c>
       <c r="C8">
-        <v>0.07481751824817519</v>
+        <v>0.0661922745321854</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>292</v>
+        <v>4819</v>
       </c>
       <c r="C9">
-        <v>0.0666058394160584</v>
+        <v>0.05851780791975811</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>258</v>
+        <v>4348</v>
       </c>
       <c r="C10">
-        <v>0.05885036496350365</v>
+        <v>0.05279838739055992</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>151</v>
+        <v>2919</v>
       </c>
       <c r="C11">
-        <v>0.03444343065693431</v>
+        <v>0.03544583550897985</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -4516,87 +3902,87 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>144</v>
+        <v>2271</v>
       </c>
       <c r="C12">
-        <v>0.03284671532846715</v>
+        <v>0.02757707860256706</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>142</v>
+        <v>2246</v>
       </c>
       <c r="C13">
-        <v>0.03239051094890511</v>
+        <v>0.02727350001821471</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>111</v>
+        <v>1658</v>
       </c>
       <c r="C14">
-        <v>0.02531934306569343</v>
+        <v>0.02013333171424755</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>48</v>
+        <v>1608</v>
       </c>
       <c r="C15">
-        <v>0.01094890510948905</v>
+        <v>0.01952617454554286</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>18</v>
+        <v>908</v>
       </c>
       <c r="C16">
-        <v>0.004105839416058394</v>
+        <v>0.01102597418367719</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>258</v>
       </c>
       <c r="C17">
-        <v>0.0006843065693430657</v>
+        <v>0.003132930990516205</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C18">
-        <v>0.0006843065693430657</v>
+        <v>0.0007164454590715353</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="C19">
-        <v>0.0004562043795620438</v>
+        <v>0.0006193003120787847</v>
       </c>
     </row>
   </sheetData>

</xml_diff>